<commit_message>
Worked on Gamesa Convertor
</commit_message>
<xml_diff>
--- a/ReportConvertor/ReportConvertor/AppInfoSheet.xlsx
+++ b/ReportConvertor/ReportConvertor/AppInfoSheet.xlsx
@@ -2,22 +2,23 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="195" windowWidth="20115" windowHeight="7620" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="315" windowWidth="20115" windowHeight="7500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="FileLocations" sheetId="4" r:id="rId1"/>
     <sheet name="Site" sheetId="1" r:id="rId2"/>
     <sheet name="Vendor General" sheetId="2" r:id="rId3"/>
     <sheet name="Values" sheetId="5" r:id="rId4"/>
+    <sheet name="Gamesa" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="106">
   <si>
     <t>Howard</t>
   </si>
@@ -266,15 +267,98 @@
   </si>
   <si>
     <t>VEN-096</t>
+  </si>
+  <si>
+    <t>Type Table</t>
+  </si>
+  <si>
+    <t>WO Type</t>
+  </si>
+  <si>
+    <t>ZPM7</t>
+  </si>
+  <si>
+    <t>ZPM2</t>
+  </si>
+  <si>
+    <t>ZPM3</t>
+  </si>
+  <si>
+    <t>ZPM4</t>
+  </si>
+  <si>
+    <t>ZPMP</t>
+  </si>
+  <si>
+    <t>ZPM1</t>
+  </si>
+  <si>
+    <t>do not import</t>
+  </si>
+  <si>
+    <t>Corrective Maintenance</t>
+  </si>
+  <si>
+    <t>Retrofit</t>
+  </si>
+  <si>
+    <t>Preventive Maintenance</t>
+  </si>
+  <si>
+    <t>Mpulse type</t>
+  </si>
+  <si>
+    <t>Task ID</t>
+  </si>
+  <si>
+    <t>PMI-004</t>
+  </si>
+  <si>
+    <t>PMI-003</t>
+  </si>
+  <si>
+    <t>PMI-002</t>
+  </si>
+  <si>
+    <t>Forced</t>
+  </si>
+  <si>
+    <t>Planned</t>
+  </si>
+  <si>
+    <t>Assets</t>
+  </si>
+  <si>
+    <t>Unplanned</t>
+  </si>
+  <si>
+    <t>02-High</t>
+  </si>
+  <si>
+    <t>03-Medium</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -298,14 +382,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -604,10 +698,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,6 +737,11 @@
         <v>65</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -649,6 +749,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -819,9 +920,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -989,6 +1091,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1045,4 +1148,165 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" t="s">
+        <v>103</v>
+      </c>
+      <c r="G5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" t="s">
+        <v>103</v>
+      </c>
+      <c r="G6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" t="s">
+        <v>103</v>
+      </c>
+      <c r="G7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finished Gamesa Convertor. No testing. Working on Writer Class
</commit_message>
<xml_diff>
--- a/ReportConvertor/ReportConvertor/AppInfoSheet.xlsx
+++ b/ReportConvertor/ReportConvertor/AppInfoSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="315" windowWidth="20115" windowHeight="7500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="315" windowWidth="20115" windowHeight="7500"/>
   </bookViews>
   <sheets>
     <sheet name="FileLocations" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="107">
   <si>
     <t>Howard</t>
   </si>
@@ -336,6 +336,9 @@
   </si>
   <si>
     <t>03-Medium</t>
+  </si>
+  <si>
+    <t>Output</t>
   </si>
 </sst>
 </file>
@@ -699,10 +702,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,6 +743,11 @@
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1155,7 +1163,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
finished excel writer and started with testing. Issues with convertor
</commit_message>
<xml_diff>
--- a/ReportConvertor/ReportConvertor/AppInfoSheet.xlsx
+++ b/ReportConvertor/ReportConvertor/AppInfoSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="315" windowWidth="20115" windowHeight="7500"/>
+    <workbookView xWindow="0" yWindow="375" windowWidth="20115" windowHeight="7440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FileLocations" sheetId="4" r:id="rId1"/>
@@ -215,9 +215,6 @@
     <t>Directory</t>
   </si>
   <si>
-    <t>C:\\Users\\vsivakumaran\\Documents\\Test c#</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -239,9 +236,6 @@
     <t>Regulatory Document</t>
   </si>
   <si>
-    <t>Regulator</t>
-  </si>
-  <si>
     <t>Planning</t>
   </si>
   <si>
@@ -339,6 +333,12 @@
   </si>
   <si>
     <t>Output</t>
+  </si>
+  <si>
+    <t>C:\\Users\\vsivakumaran\\Documents\\Test c#\\Gamesa</t>
+  </si>
+  <si>
+    <t>Regulatory</t>
   </si>
 </sst>
 </file>
@@ -704,14 +704,14 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -737,17 +737,17 @@
         <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -760,8 +760,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,7 +918,7 @@
         <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -932,7 +932,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,7 +945,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
         <v>41</v>
@@ -971,7 +971,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
         <v>36</v>
@@ -994,7 +994,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
         <v>37</v>
@@ -1014,7 +1014,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
         <v>38</v>
@@ -1034,7 +1034,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B5" t="s">
         <v>39</v>
@@ -1054,7 +1054,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B6" t="s">
         <v>40</v>
@@ -1074,7 +1074,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B7" t="s">
         <v>58</v>
@@ -1102,7 +1102,9 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1112,45 +1114,45 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
         <v>67</v>
-      </c>
-      <c r="B1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1164,7 +1166,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,138 +1181,138 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" t="s">
         <v>70</v>
-      </c>
-      <c r="E2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G6" t="s">
         <v>103</v>
-      </c>
-      <c r="G6" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>